<commit_message>
started working on Login Page automation
</commit_message>
<xml_diff>
--- a/src/main/java/resources/DemoEcommerceAutomation.xlsx
+++ b/src/main/java/resources/DemoEcommerceAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\eclipse-workspace\DemoEcommerceAutomation\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9378C-AFB9-44DD-A4CF-85569DFE4F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEF3987-A777-4721-90CB-0B17AEE33BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{43996707-DA37-4B78-BAFD-4E1A43A92AC7}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>TC_03</t>
   </si>
   <si>
-    <t>new arrival</t>
-  </si>
-  <si>
     <t>Provide Expected Product Title</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>TC_06</t>
+  </si>
+  <si>
+    <t>new arrivals</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,10 +482,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -512,26 +512,26 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>